<commit_message>
cap nhat thu ho
</commit_message>
<xml_diff>
--- a/templates/bb_theo_ca.xlsx
+++ b/templates/bb_theo_ca.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\2024\TruongLai\pmDaoTao\quanlydaotao\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2DAF3D-E95C-423C-8CE4-05CD53388C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B9FF42-BD7A-4ED9-B619-275B8A9166AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>BÁO CÁO TIẾP NHẬN HỒ SƠ</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Khóa học</t>
+  </si>
+  <si>
+    <t>Thu hộ</t>
   </si>
 </sst>
 </file>
@@ -180,6 +183,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -198,9 +204,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,136 +537,139 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7" t="s">
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
+    <row r="6" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
@@ -691,23 +697,25 @@
       <c r="O6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="R5:R6"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A3:Q3"/>

</xml_diff>